<commit_message>
Modified RunMode for Telephony Test Case
Signed-off-by: Jigar Mehta Git <jigar.digital@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>C1</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Ad2</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -577,7 +580,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>

</xml_diff>